<commit_message>
questionario docenti + studenti upload
</commit_message>
<xml_diff>
--- a/data_analysis/df_docenti.xlsx
+++ b/data_analysis/df_docenti.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AG16"/>
+  <dimension ref="A1:AH17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -523,6 +523,11 @@
           <t>turn</t>
         </is>
       </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>convivenza</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -2488,6 +2493,144 @@
       <c r="AG16" t="inlineStr">
         <is>
           <t>BR02</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2024-11-27 10:27:13</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>2024-11-27 10:53:38</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>109.112.95.6</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>1585</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>1732704819.245</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>R_2eWC9Qx590lQ5ae</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>41.8904</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>12.5126</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>anonymous</t>
+        </is>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>IT</t>
+        </is>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="T17">
+        <v>27</v>
+      </c>
+      <c r="U17">
+        <v>14</v>
+      </c>
+      <c r="V17">
+        <v>13</v>
+      </c>
+      <c r="W17">
+        <v>11</v>
+      </c>
+      <c r="X17">
+        <v>7</v>
+      </c>
+      <c r="Y17">
+        <v>4</v>
+      </c>
+      <c r="Z17" t="inlineStr">
+        <is>
+          <t>Classe abbastanza integrata e rispettosa delle regole</t>
+        </is>
+      </c>
+      <c r="AA17" t="inlineStr">
+        <is>
+          <t>Buone relazioni nel gruppo classe</t>
+        </is>
+      </c>
+      <c r="AB17" t="inlineStr">
+        <is>
+          <t>Buona partecipazione</t>
+        </is>
+      </c>
+      <c r="AC17" t="inlineStr">
+        <is>
+          <t>Buono il rispetto degli impegni scolastici</t>
+        </is>
+      </c>
+      <c r="AD17">
+        <v>4</v>
+      </c>
+      <c r="AE17" t="inlineStr">
+        <is>
+          <t>buona collaborazione</t>
+        </is>
+      </c>
+      <c r="AF17" t="inlineStr">
+        <is>
+          <t>E' una classe molto curiosa</t>
+        </is>
+      </c>
+      <c r="AG17" t="inlineStr">
+        <is>
+          <t>BR03</t>
+        </is>
+      </c>
+      <c r="AH17" t="inlineStr">
+        <is>
+          <t>Buono</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
upload docenti e studenti
</commit_message>
<xml_diff>
--- a/data_analysis/df_docenti.xlsx
+++ b/data_analysis/df_docenti.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AH17"/>
+  <dimension ref="A1:AH18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2634,6 +2634,144 @@
         </is>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2024-12-04 10:27:51</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>2024-12-04 10:32:19</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>37.159.58.54</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>268</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>1733308340.012</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>R_225qnrdRgp00Mmt</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>42.9786</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>13.871</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>anonymous</t>
+        </is>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>IT</t>
+        </is>
+      </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="T18">
+        <v>25</v>
+      </c>
+      <c r="U18">
+        <v>17</v>
+      </c>
+      <c r="V18">
+        <v>8</v>
+      </c>
+      <c r="W18">
+        <v>2</v>
+      </c>
+      <c r="X18">
+        <v>1</v>
+      </c>
+      <c r="Y18">
+        <v>1</v>
+      </c>
+      <c r="Z18" t="inlineStr">
+        <is>
+          <t>Buono</t>
+        </is>
+      </c>
+      <c r="AA18" t="inlineStr">
+        <is>
+          <t>Buono</t>
+        </is>
+      </c>
+      <c r="AB18" t="inlineStr">
+        <is>
+          <t>Buono</t>
+        </is>
+      </c>
+      <c r="AC18" t="inlineStr">
+        <is>
+          <t>Buono</t>
+        </is>
+      </c>
+      <c r="AD18">
+        <v>3</v>
+      </c>
+      <c r="AE18" t="inlineStr">
+        <is>
+          <t>Sufficiente</t>
+        </is>
+      </c>
+      <c r="AF18" t="inlineStr">
+        <is>
+          <t>Sufficiente</t>
+        </is>
+      </c>
+      <c r="AG18" t="inlineStr">
+        <is>
+          <t>BR04</t>
+        </is>
+      </c>
+      <c r="AH18" t="inlineStr">
+        <is>
+          <t>Buono</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>